<commit_message>
data(dice.report): test output.xlsx had no 'Vehicle-L' header
</commit_message>
<xml_diff>
--- a/tests/sampling/output.xlsx
+++ b/tests/sampling/output.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\ankostis\Work\co2mpas.git\tests\sampling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\co2mpas.git\tests\sampling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="35350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="35355"/>
   </bookViews>
   <sheets>
     <sheet name="dice_report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Field</t>
   </si>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -464,19 +464,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -484,7 +492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -492,7 +500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -500,7 +508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -508,7 +516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -516,7 +524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -524,7 +532,7 @@
         <v>-4.1399999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -535,7 +543,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -546,7 +554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -557,7 +565,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -568,7 +576,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -579,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -590,7 +598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -598,7 +606,7 @@
         <v>4.5599999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -606,7 +614,7 @@
         <v>-0.95</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -614,7 +622,7 @@
         <v>4.71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -622,7 +630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -630,7 +638,7 @@
         <v>18.739999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -638,7 +646,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -649,7 +657,7 @@
         <v>91.36</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>

</xml_diff>